<commit_message>
Paginas criar grupo e maleta
</commit_message>
<xml_diff>
--- a/planejamento_entregas_fintrack.xlsx
+++ b/planejamento_entregas_fintrack.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2dadff1cdd74743/UFRPE - CC/6 periodo 2021.1/WEB/FinTrack/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_202422188B6BC98CE941790BA363E77011D8B3E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9F332F9-C058-4239-B06C-22C7F1913211}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_202422188B6BC98CE941790BA363E77011D8B3E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D1089ED-1E86-4B1E-AC07-D0CC1E3AFDCD}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -159,7 +159,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,8 +174,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -263,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -281,17 +287,11 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -303,6 +303,39 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -523,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
@@ -537,12 +570,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="31.5" customHeight="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:4" ht="22.5" customHeight="1">
       <c r="A2" s="1"/>
@@ -567,84 +600,84 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="93.75" customHeight="1">
-      <c r="A4" s="5">
+      <c r="A4" s="16">
         <v>1</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="17">
         <v>37330</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="70.5" customHeight="1">
-      <c r="A5" s="5">
+      <c r="A5" s="16">
         <v>2</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="17">
         <v>37344</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="8"/>
+      <c r="D5" s="19"/>
     </row>
     <row r="6" spans="1:4" ht="88.5" customHeight="1">
-      <c r="A6" s="5">
+      <c r="A6" s="16">
         <v>3</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="17">
         <v>37351</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="61.5" customHeight="1">
-      <c r="A7" s="5">
+      <c r="A7" s="21">
         <v>4</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="22">
         <v>37365</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="24" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="111.75" customHeight="1">
-      <c r="A8" s="5">
+      <c r="A8" s="21">
         <v>5</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="22">
         <v>37379</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="24" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="90" customHeight="1">
-      <c r="A9" s="5">
+      <c r="A9" s="21">
         <v>6</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="22">
         <v>44698</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="8"/>
+      <c r="D9" s="24"/>
     </row>
     <row r="10" spans="1:4" ht="85.5" customHeight="1">
       <c r="A10" s="5">
@@ -653,54 +686,54 @@
       <c r="B10" s="6">
         <v>44712</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="8"/>
+      <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="12" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="13" spans="1:4" ht="15.75" customHeight="1">
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="19"/>
+      <c r="D13" s="28"/>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1">
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1">
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="11" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1">
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="3:4" ht="15.75" customHeight="1">
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="12" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" spans="3:4" ht="15.75" customHeight="1">
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
     </row>
     <row r="19" spans="3:4" ht="15.75" customHeight="1"/>
     <row r="20" spans="3:4" ht="15.75" customHeight="1"/>

</xml_diff>